<commit_message>
updates on currency converter and sort by low and high to price on search page
</commit_message>
<xml_diff>
--- a/relatedFiles/other files/final/Brands.xlsx
+++ b/relatedFiles/other files/final/Brands.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24527"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Web Dev\Laravel\_Developing_Phase_Project\Murarkey Single Vendor\Murarkey_single_vendor_ecommerce_with_vuexy_template\relatedFiles\other files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Web Dev\Laravel\_Developing_Phase_Project\Murarkey Single Vendor\Murarkey_single_vendor_ecommerce_with_vuexy_template\relatedFiles\other files\final\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C522DFE-C518-4E83-8378-5D0443B8479B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4129101C-C7F8-48FE-BA28-A0BDE09F6767}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="344" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="107">
   <si>
     <t>Name</t>
   </si>
@@ -49,9 +49,6 @@
     <t>Lotus</t>
   </si>
   <si>
-    <t>lotus</t>
-  </si>
-  <si>
     <t>Dove</t>
   </si>
   <si>
@@ -67,18 +64,6 @@
     <t>Olay</t>
   </si>
   <si>
-    <t>rimmel</t>
-  </si>
-  <si>
-    <t>olay</t>
-  </si>
-  <si>
-    <t>dove</t>
-  </si>
-  <si>
-    <t>lorel</t>
-  </si>
-  <si>
     <t>https://murarkey.com/wp-content/uploads/2020/04/WhatsApp-Image-2020-04-04-at-1.40.48-PM-6.jpeg</t>
   </si>
   <si>
@@ -88,9 +73,6 @@
     <t>Nivea</t>
   </si>
   <si>
-    <t>nivea</t>
-  </si>
-  <si>
     <t>https://demo.murarkey.com/image/cache/600X600/wzaqd56M8jhPKJCdpPkvwc70HjvhvFjFedjLbyjc.jpg</t>
   </si>
   <si>
@@ -98,12 +80,6 @@
   </si>
   <si>
     <t>Maybelline</t>
-  </si>
-  <si>
-    <t>himalaya</t>
-  </si>
-  <si>
-    <t>maybelline</t>
   </si>
   <si>
     <t>https://marcommnews.com/wp-content/uploads/2018/09/wholesale-rimmel-london-cosmetics-front-photo-wholesale55-gcbblth-7-701x394.jpg</t>
@@ -730,7 +706,7 @@
   <dimension ref="A1:D86"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection sqref="A1:D86"/>
+      <selection activeCell="B2" sqref="B2:B86"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -758,1190 +734,1275 @@
       <c r="A2" t="s">
         <v>5</v>
       </c>
-      <c r="B2" t="s">
-        <v>6</v>
+      <c r="B2" t="str">
+        <f>LOWER(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(TRIM(A2)," ","-"),"'",""),"""",""),"/",""),"?",""),".",""),"&gt;",""),"&lt;",""),",",""),";",""),":",""),"[",""),"]",""),"}",""),"[",""),"{",""),"|",""),"\",""),"+",""),"=",""),"~",""),"`",""),"!",""),"@",""),"#",""),"$",""),"%",""),"^",""),"&amp;",""),"*",""),"(",""),")",""),"#",""),"'",""),"""",""),"---","-"),"--","-"))</f>
+        <v>lotus</v>
       </c>
       <c r="C2" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>18</v>
-      </c>
-      <c r="B3" t="s">
-        <v>19</v>
+        <v>13</v>
+      </c>
+      <c r="B3" t="str">
+        <f t="shared" ref="B3:B66" si="0">LOWER(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(TRIM(A3)," ","-"),"'",""),"""",""),"/",""),"?",""),".",""),"&gt;",""),"&lt;",""),",",""),";",""),":",""),"[",""),"]",""),"}",""),"[",""),"{",""),"|",""),"\",""),"+",""),"=",""),"~",""),"`",""),"!",""),"@",""),"#",""),"$",""),"%",""),"^",""),"&amp;",""),"*",""),"(",""),")",""),"#",""),"'",""),"""",""),"---","-"),"--","-"))</f>
+        <v>nivea</v>
       </c>
       <c r="C3" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="D3" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4" t="s">
-        <v>14</v>
+        <v>6</v>
+      </c>
+      <c r="B4" t="str">
+        <f t="shared" si="0"/>
+        <v>dove</v>
       </c>
       <c r="C4" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="D4" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>23</v>
+        <v>7</v>
+      </c>
+      <c r="B5" t="str">
+        <f t="shared" si="0"/>
+        <v>himalaya</v>
       </c>
       <c r="C5" t="s">
         <v>4</v>
       </c>
       <c r="D5" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>9</v>
-      </c>
-      <c r="B6" t="s">
-        <v>15</v>
+        <v>8</v>
+      </c>
+      <c r="B6" t="str">
+        <f t="shared" si="0"/>
+        <v>lorel</v>
       </c>
       <c r="C6" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="D6" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>22</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>24</v>
+        <v>16</v>
+      </c>
+      <c r="B7" t="str">
+        <f t="shared" si="0"/>
+        <v>maybelline</v>
       </c>
       <c r="C7" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>10</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>12</v>
+        <v>9</v>
+      </c>
+      <c r="B8" t="str">
+        <f t="shared" si="0"/>
+        <v>rimmel</v>
       </c>
       <c r="C8" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="D8" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>11</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>13</v>
+        <v>10</v>
+      </c>
+      <c r="B9" t="str">
+        <f t="shared" si="0"/>
+        <v>olay</v>
       </c>
       <c r="C9" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="D9" t="s">
-        <v>33</v>
+        <v>25</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>71</v>
-      </c>
-      <c r="B10" t="s">
-        <v>71</v>
+        <v>63</v>
+      </c>
+      <c r="B10" t="str">
+        <f t="shared" si="0"/>
+        <v>aekyung</v>
       </c>
       <c r="C10" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="D10" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>74</v>
-      </c>
-      <c r="B11" t="s">
-        <v>74</v>
+        <v>66</v>
+      </c>
+      <c r="B11" t="str">
+        <f t="shared" si="0"/>
+        <v>amayra</v>
       </c>
       <c r="C11" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="D11" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>41</v>
-      </c>
-      <c r="B12" t="s">
-        <v>41</v>
+        <v>33</v>
+      </c>
+      <c r="B12" t="str">
+        <f t="shared" si="0"/>
+        <v>astaberry</v>
       </c>
       <c r="C12" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="D12" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>38</v>
-      </c>
-      <c r="B13" t="s">
-        <v>38</v>
+        <v>30</v>
+      </c>
+      <c r="B13" t="str">
+        <f t="shared" si="0"/>
+        <v>beardo</v>
       </c>
       <c r="C13" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="D13" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>75</v>
-      </c>
-      <c r="B14" t="s">
-        <v>75</v>
+        <v>67</v>
+      </c>
+      <c r="B14" t="str">
+        <f t="shared" si="0"/>
+        <v>bella</v>
       </c>
       <c r="C14" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="D14" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>47</v>
-      </c>
-      <c r="B15" t="s">
-        <v>47</v>
+        <v>39</v>
+      </c>
+      <c r="B15" t="str">
+        <f t="shared" si="0"/>
+        <v>bella-vita</v>
       </c>
       <c r="C15" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="D15" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>46</v>
-      </c>
-      <c r="B16" t="s">
-        <v>46</v>
+        <v>38</v>
+      </c>
+      <c r="B16" t="str">
+        <f t="shared" si="0"/>
+        <v>biotique</v>
       </c>
       <c r="C16" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="D16" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>63</v>
-      </c>
-      <c r="B17" t="s">
-        <v>63</v>
+        <v>55</v>
+      </c>
+      <c r="B17" t="str">
+        <f t="shared" si="0"/>
+        <v>blue-tree</v>
       </c>
       <c r="C17" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="D17" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>76</v>
-      </c>
-      <c r="B18" t="s">
-        <v>76</v>
+        <v>68</v>
+      </c>
+      <c r="B18" t="str">
+        <f t="shared" si="0"/>
+        <v>brillare-science</v>
       </c>
       <c r="C18" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="D18" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>70</v>
-      </c>
-      <c r="B19" t="s">
-        <v>70</v>
+        <v>62</v>
+      </c>
+      <c r="B19" t="str">
+        <f t="shared" si="0"/>
+        <v>by-vilain</v>
       </c>
       <c r="C19" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="D19" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>49</v>
-      </c>
-      <c r="B20" t="s">
-        <v>49</v>
+        <v>41</v>
+      </c>
+      <c r="B20" t="str">
+        <f t="shared" si="0"/>
+        <v>cerave</v>
       </c>
       <c r="C20" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="D20" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>40</v>
-      </c>
-      <c r="B21" t="s">
-        <v>40</v>
+        <v>32</v>
+      </c>
+      <c r="B21" t="str">
+        <f t="shared" si="0"/>
+        <v>cetaphil</v>
       </c>
       <c r="C21" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="D21" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>77</v>
-      </c>
-      <c r="B22" t="s">
-        <v>77</v>
+        <v>69</v>
+      </c>
+      <c r="B22" t="str">
+        <f t="shared" si="0"/>
+        <v>clovia-botaniqa</v>
       </c>
       <c r="C22" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="D22" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>78</v>
-      </c>
-      <c r="B23" t="s">
-        <v>78</v>
+        <v>70</v>
+      </c>
+      <c r="B23" t="str">
+        <f t="shared" si="0"/>
+        <v>diva</v>
       </c>
       <c r="C23" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="D23" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>79</v>
-      </c>
-      <c r="B24" t="s">
-        <v>79</v>
+        <v>71</v>
+      </c>
+      <c r="B24" t="str">
+        <f t="shared" si="0"/>
+        <v>doers-of-london</v>
       </c>
       <c r="C24" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="D24" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>39</v>
-      </c>
-      <c r="B25" t="s">
-        <v>39</v>
+        <v>31</v>
+      </c>
+      <c r="B25" t="str">
+        <f t="shared" si="0"/>
+        <v>earth-rhythm</v>
       </c>
       <c r="C25" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="D25" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>80</v>
-      </c>
-      <c r="B26" t="s">
-        <v>80</v>
+        <v>72</v>
+      </c>
+      <c r="B26" t="str">
+        <f t="shared" si="0"/>
+        <v>emami</v>
       </c>
       <c r="C26" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="D26" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>81</v>
-      </c>
-      <c r="B27" t="s">
-        <v>81</v>
+        <v>73</v>
+      </c>
+      <c r="B27" t="str">
+        <f t="shared" si="0"/>
+        <v>essence-of-life</v>
       </c>
       <c r="C27" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="D27" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>68</v>
-      </c>
-      <c r="B28" t="s">
-        <v>68</v>
+        <v>60</v>
+      </c>
+      <c r="B28" t="str">
+        <f t="shared" si="0"/>
+        <v>everteen</v>
       </c>
       <c r="C28" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="D28" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>44</v>
-      </c>
-      <c r="B29" t="s">
-        <v>44</v>
+        <v>36</v>
+      </c>
+      <c r="B29" t="str">
+        <f t="shared" si="0"/>
+        <v>farmasi</v>
       </c>
       <c r="C29" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="D29" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>82</v>
-      </c>
-      <c r="B30" t="s">
-        <v>82</v>
+        <v>74</v>
+      </c>
+      <c r="B30" t="str">
+        <f t="shared" si="0"/>
+        <v>future-organics</v>
       </c>
       <c r="C30" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="D30" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>69</v>
-      </c>
-      <c r="B31" t="s">
-        <v>69</v>
+        <v>61</v>
+      </c>
+      <c r="B31" t="str">
+        <f t="shared" si="0"/>
+        <v>hanz-de-fuko</v>
       </c>
       <c r="C31" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="D31" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>83</v>
-      </c>
-      <c r="B32" t="s">
-        <v>83</v>
+        <v>75</v>
+      </c>
+      <c r="B32" t="str">
+        <f t="shared" si="0"/>
+        <v>head-shoulders</v>
       </c>
       <c r="C32" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="D32" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>60</v>
-      </c>
-      <c r="B33" t="s">
-        <v>60</v>
+        <v>52</v>
+      </c>
+      <c r="B33" t="str">
+        <f t="shared" si="0"/>
+        <v>himalayan-bio</v>
       </c>
       <c r="C33" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="D33" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>84</v>
-      </c>
-      <c r="B34" t="s">
-        <v>84</v>
+        <v>76</v>
+      </c>
+      <c r="B34" t="str">
+        <f t="shared" si="0"/>
+        <v>jina-alchemy</v>
       </c>
       <c r="C34" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="D34" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>85</v>
-      </c>
-      <c r="B35" t="s">
-        <v>85</v>
+        <v>77</v>
+      </c>
+      <c r="B35" t="str">
+        <f t="shared" si="0"/>
+        <v>joy</v>
       </c>
       <c r="C35" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="D35" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>58</v>
-      </c>
-      <c r="B36" t="s">
-        <v>58</v>
+        <v>50</v>
+      </c>
+      <c r="B36" t="str">
+        <f t="shared" si="0"/>
+        <v>juas</v>
       </c>
       <c r="C36" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="D36" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>86</v>
-      </c>
-      <c r="B37" t="s">
-        <v>86</v>
+        <v>78</v>
+      </c>
+      <c r="B37" t="str">
+        <f t="shared" si="0"/>
+        <v>juicy</v>
       </c>
       <c r="C37" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="D37" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>61</v>
-      </c>
-      <c r="B38" t="s">
-        <v>61</v>
+        <v>53</v>
+      </c>
+      <c r="B38" t="str">
+        <f t="shared" si="0"/>
+        <v>juicy-chemistry</v>
       </c>
       <c r="C38" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="D38" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>87</v>
-      </c>
-      <c r="B39" t="s">
-        <v>87</v>
+        <v>79</v>
+      </c>
+      <c r="B39" t="str">
+        <f t="shared" si="0"/>
+        <v>kaimono</v>
       </c>
       <c r="C39" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="D39" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>88</v>
-      </c>
-      <c r="B40" t="s">
-        <v>88</v>
+        <v>80</v>
+      </c>
+      <c r="B40" t="str">
+        <f t="shared" si="0"/>
+        <v>kaimono-japan</v>
       </c>
       <c r="C40" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="D40" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>56</v>
-      </c>
-      <c r="B41" t="s">
-        <v>56</v>
+        <v>48</v>
+      </c>
+      <c r="B41" t="str">
+        <f t="shared" si="0"/>
+        <v>kanti-herbal</v>
       </c>
       <c r="C41" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="D41" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>89</v>
-      </c>
-      <c r="B42" t="s">
-        <v>89</v>
+        <v>81</v>
+      </c>
+      <c r="B42" t="str">
+        <f t="shared" si="0"/>
+        <v>kesh-king</v>
       </c>
       <c r="C42" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="D42" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>65</v>
-      </c>
-      <c r="B43" t="s">
-        <v>65</v>
+        <v>57</v>
+      </c>
+      <c r="B43" t="str">
+        <f t="shared" si="0"/>
+        <v>khadi-naturals</v>
       </c>
       <c r="C43" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="D43" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>90</v>
-      </c>
-      <c r="B44" t="s">
-        <v>90</v>
+        <v>82</v>
+      </c>
+      <c r="B44" t="str">
+        <f t="shared" si="0"/>
+        <v>lae-sa-luay</v>
       </c>
       <c r="C44" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="D44" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>67</v>
-      </c>
-      <c r="B45" t="s">
-        <v>67</v>
+        <v>59</v>
+      </c>
+      <c r="B45" t="str">
+        <f t="shared" si="0"/>
+        <v>lakme</v>
       </c>
       <c r="C45" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="D45" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>91</v>
-      </c>
-      <c r="B46" t="s">
-        <v>91</v>
+        <v>83</v>
+      </c>
+      <c r="B46" t="str">
+        <f t="shared" si="0"/>
+        <v>lisap</v>
       </c>
       <c r="C46" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="D46" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>92</v>
-      </c>
-      <c r="B47" t="s">
-        <v>92</v>
+        <v>84</v>
+      </c>
+      <c r="B47" t="str">
+        <f t="shared" si="0"/>
+        <v>loreal</v>
       </c>
       <c r="C47" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="D47" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>37</v>
-      </c>
-      <c r="B48" t="s">
-        <v>37</v>
+        <v>29</v>
+      </c>
+      <c r="B48" t="str">
+        <f t="shared" si="0"/>
+        <v>mamaearth</v>
       </c>
       <c r="C48" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="D48" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>93</v>
-      </c>
-      <c r="B49" t="s">
-        <v>93</v>
+        <v>85</v>
+      </c>
+      <c r="B49" t="str">
+        <f t="shared" si="0"/>
+        <v>modicare</v>
       </c>
       <c r="C49" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="D49" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>64</v>
-      </c>
-      <c r="B50" t="s">
-        <v>64</v>
+        <v>56</v>
+      </c>
+      <c r="B50" t="str">
+        <f t="shared" si="0"/>
+        <v>moonwake</v>
       </c>
       <c r="C50" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="D50" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>94</v>
-      </c>
-      <c r="B51" t="s">
-        <v>94</v>
+        <v>86</v>
+      </c>
+      <c r="B51" t="str">
+        <f t="shared" si="0"/>
+        <v>myglamm</v>
       </c>
       <c r="C51" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="D51" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>95</v>
-      </c>
-      <c r="B52" t="s">
-        <v>95</v>
+        <v>87</v>
+      </c>
+      <c r="B52" t="str">
+        <f t="shared" si="0"/>
+        <v>mysa</v>
       </c>
       <c r="C52" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="D52" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>55</v>
-      </c>
-      <c r="B53" t="s">
-        <v>55</v>
+        <v>47</v>
+      </c>
+      <c r="B53" t="str">
+        <f t="shared" si="0"/>
+        <v>natures-essence</v>
       </c>
       <c r="C53" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="D53" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>96</v>
-      </c>
-      <c r="B54" t="s">
-        <v>96</v>
+        <v>88</v>
+      </c>
+      <c r="B54" t="str">
+        <f t="shared" si="0"/>
+        <v>natures-tattva</v>
       </c>
       <c r="C54" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="D54" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>59</v>
-      </c>
-      <c r="B55" t="s">
-        <v>59</v>
+        <v>51</v>
+      </c>
+      <c r="B55" t="str">
+        <f t="shared" si="0"/>
+        <v>naturo-earth</v>
       </c>
       <c r="C55" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="D55" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>97</v>
-      </c>
-      <c r="B56" t="s">
-        <v>97</v>
+        <v>89</v>
+      </c>
+      <c r="B56" t="str">
+        <f t="shared" si="0"/>
+        <v>neud</v>
       </c>
       <c r="C56" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="D56" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>50</v>
-      </c>
-      <c r="B57" t="s">
-        <v>50</v>
+        <v>42</v>
+      </c>
+      <c r="B57" t="str">
+        <f t="shared" si="0"/>
+        <v>neutrogena</v>
       </c>
       <c r="C57" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="D57" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>98</v>
-      </c>
-      <c r="B58" t="s">
-        <v>98</v>
+        <v>90</v>
+      </c>
+      <c r="B58" t="str">
+        <f t="shared" si="0"/>
+        <v>newlook</v>
       </c>
       <c r="C58" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="D58" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>99</v>
-      </c>
-      <c r="B59" t="s">
-        <v>99</v>
+        <v>91</v>
+      </c>
+      <c r="B59" t="str">
+        <f t="shared" si="0"/>
+        <v>no-brand</v>
       </c>
       <c r="C59" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="D59" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>45</v>
-      </c>
-      <c r="B60" t="s">
-        <v>45</v>
+        <v>37</v>
+      </c>
+      <c r="B60" t="str">
+        <f t="shared" si="0"/>
+        <v>oriflame</v>
       </c>
       <c r="C60" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="D60" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>100</v>
-      </c>
-      <c r="B61" t="s">
-        <v>100</v>
+        <v>92</v>
+      </c>
+      <c r="B61" t="str">
+        <f t="shared" si="0"/>
+        <v>pantene</v>
       </c>
       <c r="C61" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="D61" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>66</v>
-      </c>
-      <c r="B62" t="s">
-        <v>66</v>
+        <v>58</v>
+      </c>
+      <c r="B62" t="str">
+        <f t="shared" si="0"/>
+        <v>pee-safe</v>
       </c>
       <c r="C62" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="D62" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>101</v>
-      </c>
-      <c r="B63" t="s">
-        <v>101</v>
+        <v>93</v>
+      </c>
+      <c r="B63" t="str">
+        <f t="shared" si="0"/>
+        <v>phy</v>
       </c>
       <c r="C63" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="D63" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>51</v>
-      </c>
-      <c r="B64" t="s">
-        <v>51</v>
+        <v>43</v>
+      </c>
+      <c r="B64" t="str">
+        <f t="shared" si="0"/>
+        <v>plum</v>
       </c>
       <c r="C64" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="D64" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>102</v>
-      </c>
-      <c r="B65" t="s">
-        <v>102</v>
+        <v>94</v>
+      </c>
+      <c r="B65" t="str">
+        <f t="shared" si="0"/>
+        <v>plum-goodness</v>
       </c>
       <c r="C65" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="D65" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>103</v>
-      </c>
-      <c r="B66" t="s">
-        <v>103</v>
+        <v>95</v>
+      </c>
+      <c r="B66" t="str">
+        <f t="shared" si="0"/>
+        <v>pump-haircare</v>
       </c>
       <c r="C66" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="D66" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>104</v>
-      </c>
-      <c r="B67" t="s">
-        <v>104</v>
+        <v>96</v>
+      </c>
+      <c r="B67" t="str">
+        <f t="shared" ref="B67:B86" si="1">LOWER(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(TRIM(A67)," ","-"),"'",""),"""",""),"/",""),"?",""),".",""),"&gt;",""),"&lt;",""),",",""),";",""),":",""),"[",""),"]",""),"}",""),"[",""),"{",""),"|",""),"\",""),"+",""),"=",""),"~",""),"`",""),"!",""),"@",""),"#",""),"$",""),"%",""),"^",""),"&amp;",""),"*",""),"(",""),")",""),"#",""),"'",""),"""",""),"---","-"),"--","-"))</f>
+        <v>revlon</v>
       </c>
       <c r="C67" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="D67" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>105</v>
-      </c>
-      <c r="B68" t="s">
-        <v>105</v>
+        <v>97</v>
+      </c>
+      <c r="B68" t="str">
+        <f t="shared" si="1"/>
+        <v>rustic-art</v>
       </c>
       <c r="C68" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="D68" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>62</v>
-      </c>
-      <c r="B69" t="s">
-        <v>62</v>
+        <v>54</v>
+      </c>
+      <c r="B69" t="str">
+        <f t="shared" si="1"/>
+        <v>saanjh</v>
       </c>
       <c r="C69" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="D69" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>42</v>
-      </c>
-      <c r="B70" t="s">
-        <v>42</v>
+        <v>34</v>
+      </c>
+      <c r="B70" t="str">
+        <f t="shared" si="1"/>
+        <v>sara-food</v>
       </c>
       <c r="C70" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="D70" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>57</v>
-      </c>
-      <c r="B71" t="s">
-        <v>57</v>
+        <v>49</v>
+      </c>
+      <c r="B71" t="str">
+        <f t="shared" si="1"/>
+        <v>sara-foods</v>
       </c>
       <c r="C71" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="D71" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>48</v>
-      </c>
-      <c r="B72" t="s">
-        <v>48</v>
+        <v>40</v>
+      </c>
+      <c r="B72" t="str">
+        <f t="shared" si="1"/>
+        <v>sebamed</v>
       </c>
       <c r="C72" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="D72" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>106</v>
-      </c>
-      <c r="B73" t="s">
-        <v>106</v>
+        <v>98</v>
+      </c>
+      <c r="B73" t="str">
+        <f t="shared" si="1"/>
+        <v>selsun</v>
       </c>
       <c r="C73" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="D73" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>107</v>
-      </c>
-      <c r="B74" t="s">
-        <v>107</v>
+        <v>99</v>
+      </c>
+      <c r="B74" t="str">
+        <f t="shared" si="1"/>
+        <v>soapworks</v>
       </c>
       <c r="C74" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="D74" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>108</v>
-      </c>
-      <c r="B75" t="s">
-        <v>108</v>
+        <v>100</v>
+      </c>
+      <c r="B75" t="str">
+        <f t="shared" si="1"/>
+        <v>soultree</v>
       </c>
       <c r="C75" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="D75" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>109</v>
-      </c>
-      <c r="B76" t="s">
-        <v>109</v>
+        <v>101</v>
+      </c>
+      <c r="B76" t="str">
+        <f t="shared" si="1"/>
+        <v>the-beard-story</v>
       </c>
       <c r="C76" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="D76" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>43</v>
-      </c>
-      <c r="B77" t="s">
-        <v>43</v>
+        <v>35</v>
+      </c>
+      <c r="B77" t="str">
+        <f t="shared" si="1"/>
+        <v>the-derma</v>
       </c>
       <c r="C77" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="D77" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>110</v>
-      </c>
-      <c r="B78" t="s">
-        <v>110</v>
+        <v>102</v>
+      </c>
+      <c r="B78" t="str">
+        <f t="shared" si="1"/>
+        <v>the-moms-co</v>
       </c>
       <c r="C78" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="D78" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>111</v>
-      </c>
-      <c r="B79" t="s">
-        <v>111</v>
+        <v>103</v>
+      </c>
+      <c r="B79" t="str">
+        <f t="shared" si="1"/>
+        <v>the-skin-story</v>
       </c>
       <c r="C79" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="D79" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>112</v>
-      </c>
-      <c r="B80" t="s">
-        <v>112</v>
+        <v>104</v>
+      </c>
+      <c r="B80" t="str">
+        <f t="shared" si="1"/>
+        <v>tresemme</v>
       </c>
       <c r="C80" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="D80" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>113</v>
-      </c>
-      <c r="B81" t="s">
-        <v>113</v>
+        <v>105</v>
+      </c>
+      <c r="B81" t="str">
+        <f t="shared" si="1"/>
+        <v>ustraa</v>
       </c>
       <c r="C81" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="D81" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>36</v>
-      </c>
-      <c r="B82" t="s">
-        <v>36</v>
+        <v>28</v>
+      </c>
+      <c r="B82" t="str">
+        <f t="shared" si="1"/>
+        <v>usupso</v>
       </c>
       <c r="C82" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="D82" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>54</v>
-      </c>
-      <c r="B83" t="s">
-        <v>54</v>
+        <v>46</v>
+      </c>
+      <c r="B83" t="str">
+        <f t="shared" si="1"/>
+        <v>victorias-secret</v>
       </c>
       <c r="C83" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="D83" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>52</v>
-      </c>
-      <c r="B84" t="s">
-        <v>52</v>
+        <v>44</v>
+      </c>
+      <c r="B84" t="str">
+        <f t="shared" si="1"/>
+        <v>wild-earth</v>
       </c>
       <c r="C84" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="D84" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>53</v>
-      </c>
-      <c r="B85" t="s">
-        <v>53</v>
+        <v>45</v>
+      </c>
+      <c r="B85" t="str">
+        <f t="shared" si="1"/>
+        <v>ximi</v>
       </c>
       <c r="C85" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="D85" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>114</v>
-      </c>
-      <c r="B86" t="s">
-        <v>114</v>
+        <v>106</v>
+      </c>
+      <c r="B86" t="str">
+        <f t="shared" si="1"/>
+        <v>yoyoso</v>
       </c>
       <c r="C86" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="D86" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
     </row>
   </sheetData>

</xml_diff>